<commit_message>
Update: Fix new logic for import data
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\assetManagement-app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naufal Ammar H\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590A655-779D-4016-ABBC-802F09CE387D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F75EDA0-D6A6-4FBB-A782-17FEAE450C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Kode Asset Lama</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Nilai Perolehan</t>
+  </si>
+  <si>
+    <t>Merk</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Dept</t>
   </si>
 </sst>
 </file>
@@ -157,9 +166,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,7 +206,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -303,7 +312,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,27 +462,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7210F671-66B7-488E-9E23-21BC8C84AFDD}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.23046875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.69140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.07421875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.84375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.53515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.3046875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.84375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,22 +498,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Add status in excel
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naufal Ammar H\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\AssetManagement\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F75EDA0-D6A6-4FBB-A782-17FEAE450C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2F2DB-1C04-40D2-9BD5-D01F6B86218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{C3BC6170-B98B-4206-89CA-6E150A74B46C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Kode Asset Lama</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Dept</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7210F671-66B7-488E-9E23-21BC8C84AFDD}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -480,11 +483,11 @@
     <col min="8" max="8" width="20.53515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="20.3046875" style="4" customWidth="1"/>
     <col min="10" max="10" width="21.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="21.84375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.765625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="21.84375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.765625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,9 +522,12 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>